<commit_message>
Added form mattrix mapping.
</commit_message>
<xml_diff>
--- a/generated-output.xlsx
+++ b/generated-output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="23">
   <si>
     <t>S.no</t>
   </si>
@@ -34,16 +34,16 @@
     <t>Repository</t>
   </si>
   <si>
-    <t>TC_1_Verify the dynamic fields for CA 11 211</t>
-  </si>
-  <si>
-    <t>Verify the dynamic fields for CA 11 211</t>
+    <t>TC_1_Verify the dynamic fields for BAS UM (GA) 12 49 - Georgia Manhole Liability Coverage</t>
+  </si>
+  <si>
+    <t>Verify the dynamic fields for BAS UM (GA) 12 49 - Georgia Manhole Liability Coverage</t>
   </si>
   <si>
     <t>Manual</t>
   </si>
   <si>
-    <t>Login to PC and initiate a submission</t>
+    <t>Login to PC and initiate a submission for GA</t>
   </si>
   <si>
     <t>User should be able to log in successfully and should be navigated to the Home Screen</t>
@@ -61,10 +61,10 @@
     <t>User should be able to start a New submission transaction</t>
   </si>
   <si>
-    <t>Navigate to COVERAGE_TYPE tab.</t>
-  </si>
-  <si>
-    <t>User should be able to nanvigate to the COVERAGE_TYPE screen</t>
+    <t>Add  will triggered when Manhole Liability coverage is selected</t>
+  </si>
+  <si>
+    <t>User should be able to add all the terms</t>
   </si>
   <si>
     <t>Verify that the below Coverage Term(s) is(are) displayed FIELDS</t>
@@ -73,10 +73,13 @@
     <t>The Coverage Term(s) should be displayed along with the default value (if any) and options available for selection</t>
   </si>
   <si>
-    <t>TC_1_Verify the dynamic fields for BA 15 210</t>
-  </si>
-  <si>
-    <t>Verify the dynamic fields for BA 15 210</t>
+    <t>TC_1_Verify the dynamic fields for BAS UM (AZ) 03 12 - Arizona Manhole Liability Coverage</t>
+  </si>
+  <si>
+    <t>Verify the dynamic fields for BAS UM (AZ) 03 12 - Arizona Manhole Liability Coverage</t>
+  </si>
+  <si>
+    <t>Login to PC and initiate a submission for AZ</t>
   </si>
 </sst>
 </file>
@@ -95,15 +98,12 @@
       <b/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid"/>
     </fill>
   </fills>
   <borders count="1">
@@ -120,7 +120,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,8 +464,7 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="2" max="3" width="50" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="6" width="50" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
@@ -600,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>

</xml_diff>